<commit_message>
save details and back button
</commit_message>
<xml_diff>
--- a/Documentation/Finance.xlsx
+++ b/Documentation/Finance.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamvr\Desktop\cerberus-web\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10455"/>
   </bookViews>
   <sheets>
     <sheet name="Finance" sheetId="1" r:id="rId1"/>
     <sheet name="Quotation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>Fingerprint Sensor</t>
   </si>
@@ -236,13 +231,16 @@
   </si>
   <si>
     <t>Sheet cutting</t>
+  </si>
+  <si>
+    <t>Box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,7 +683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -720,7 +718,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -897,22 +895,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
@@ -926,7 +924,7 @@
     <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -946,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="10">
         <v>43571</v>
       </c>
@@ -967,7 +965,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="10">
         <v>43571</v>
       </c>
@@ -988,7 +986,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="10">
         <v>43572</v>
       </c>
@@ -1009,7 +1007,7 @@
         <v>810.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="10">
         <v>43579</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="10">
         <v>43581</v>
       </c>
@@ -1060,7 +1058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="10">
         <v>43581</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="14">
         <v>43584</v>
       </c>
@@ -1102,7 +1100,7 @@
         <v>-202.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="10">
         <v>43584</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="10">
         <v>43587</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -1150,7 +1148,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1171,8 +1169,8 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="15" spans="1:10">
       <c r="A15" s="10">
         <v>43596</v>
       </c>
@@ -1193,7 +1191,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="10">
         <v>43596</v>
       </c>
@@ -1214,7 +1212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="10">
         <v>43597</v>
       </c>
@@ -1235,7 +1233,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="10">
         <v>43600</v>
       </c>
@@ -1256,7 +1254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="10">
         <v>43600</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
       <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
@@ -1294,8 +1292,8 @@
         <v>387</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" thickTop="1"/>
+    <row r="24" spans="1:6">
       <c r="A24" s="10">
         <v>43603</v>
       </c>
@@ -1316,7 +1314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="10">
         <v>43603</v>
       </c>
@@ -1337,7 +1335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="10">
         <v>43603</v>
       </c>
@@ -1358,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="10">
         <v>43603</v>
       </c>
@@ -1379,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="10">
         <v>43603</v>
       </c>
@@ -1400,7 +1398,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="10">
         <v>43603</v>
       </c>
@@ -1421,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1">
       <c r="B31" s="19" t="s">
         <v>20</v>
       </c>
@@ -1438,8 +1436,8 @@
         <v>58.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" thickTop="1"/>
+    <row r="33" spans="1:8">
       <c r="B33" s="29" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1446,7 @@
         <v>4739</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="37" customFormat="1">
       <c r="B34" s="25" t="s">
         <v>61</v>
       </c>
@@ -1456,7 +1454,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15.75" thickBot="1">
       <c r="B35" s="33" t="s">
         <v>62</v>
       </c>
@@ -1465,13 +1463,13 @@
         <v>4809</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15.75" thickTop="1"/>
+    <row r="38" spans="1:8">
       <c r="B38" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="B39" s="11" t="s">
         <v>32</v>
       </c>
@@ -1481,7 +1479,7 @@
       </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="B40" s="30" t="s">
         <v>33</v>
       </c>
@@ -1496,10 +1494,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="28"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +1520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="10">
         <v>43735</v>
       </c>
@@ -1546,7 +1544,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="10">
         <v>43735</v>
       </c>
@@ -1570,7 +1568,7 @@
         <v>16.333333333333332</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="35">
         <v>43735</v>
       </c>
@@ -1596,7 +1594,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="10">
         <v>43735</v>
       </c>
@@ -1620,7 +1618,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="B49" s="34" t="s">
         <v>20</v>
       </c>
@@ -1637,7 +1635,7 @@
         <v>676.33333333333326</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
@@ -1646,7 +1644,7 @@
         <v>2279.333333333333</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="8" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1668,7 @@
       </c>
       <c r="I54" s="37"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="10">
         <v>43735</v>
       </c>
@@ -1694,7 +1692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="10">
         <v>43735</v>
       </c>
@@ -1718,7 +1716,7 @@
         <v>13.333333333333334</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="10">
         <v>43735</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="10">
         <v>43735</v>
       </c>
@@ -1766,7 +1764,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="10">
         <v>43735</v>
       </c>
@@ -1790,7 +1788,7 @@
         <v>36.666666666666664</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="C61" s="40">
         <f>SUM(C55:C59)</f>
         <v>625</v>
@@ -1800,8 +1798,8 @@
         <v>208.33333333333334</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="64" spans="1:9" ht="15.75" thickBot="1">
       <c r="B64" s="33" t="s">
         <v>21</v>
       </c>
@@ -1810,7 +1808,7 @@
         <v>7463</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15.75" thickTop="1">
       <c r="B65" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="B66" s="38" t="s">
         <v>32</v>
       </c>
@@ -1830,7 +1828,7 @@
         <v>2487.6666666666665</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="B67" t="s">
         <v>44</v>
       </c>
@@ -1840,7 +1838,7 @@
       </c>
       <c r="H67" s="26"/>
     </row>
-    <row r="68" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" s="45" customFormat="1">
       <c r="B68" t="s">
         <v>45</v>
       </c>
@@ -1850,7 +1848,7 @@
       </c>
       <c r="H68" s="26"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8" t="s">
         <v>8</v>
       </c>
@@ -1873,7 +1871,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="10">
         <v>43774</v>
       </c>
@@ -1883,10 +1881,7 @@
       <c r="C72" s="47">
         <v>100</v>
       </c>
-      <c r="D72" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="47">
+      <c r="D72" s="47">
         <v>100</v>
       </c>
       <c r="F72" s="47" t="s">
@@ -1897,7 +1892,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="10">
         <v>43775</v>
       </c>
@@ -1905,65 +1900,74 @@
         <v>71</v>
       </c>
       <c r="C73" s="47">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
+      <c r="E73" s="47">
+        <v>150</v>
+      </c>
       <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G73" s="50">
+        <f>C73/3</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="C75" s="51">
         <f>SUM(C72:C73)</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="G75" s="23">
+        <f>SUM(G72:G73)</f>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1">
       <c r="B78" s="33" t="s">
         <v>21</v>
       </c>
       <c r="C78" s="49">
         <f>C35+C49+C61+C75</f>
-        <v>7564</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>7713</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" thickTop="1">
       <c r="B79" s="45" t="s">
         <v>43</v>
       </c>
       <c r="C79" s="45">
-        <v>4419</v>
+        <v>4620</v>
       </c>
       <c r="D79" s="45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="B80" s="47" t="s">
         <v>32</v>
       </c>
       <c r="C80" s="52">
         <f>C78/3</f>
-        <v>2521.3333333333335</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
       <c r="B81" s="53" t="s">
         <v>44</v>
       </c>
       <c r="C81">
         <f>C78-C79</f>
-        <v>3145</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
       <c r="B82" s="45" t="s">
         <v>45</v>
       </c>
       <c r="C82">
         <f>C81/3</f>
-        <v>1048.3333333333333</v>
+        <v>1031</v>
       </c>
     </row>
   </sheetData>
@@ -1973,26 +1977,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="43" customFormat="1">
       <c r="A2" s="46" t="s">
         <v>47</v>
       </c>
@@ -2003,7 +2007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="44" t="s">
         <v>36</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="44" t="s">
         <v>37</v>
       </c>
@@ -2025,7 +2029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="44" t="s">
         <v>50</v>
       </c>
@@ -2036,7 +2040,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="44" t="s">
         <v>51</v>
       </c>
@@ -2047,7 +2051,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="48" t="s">
         <v>29</v>
       </c>
@@ -2058,7 +2062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="44" t="s">
         <v>52</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="48" t="s">
         <v>53</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="44" t="s">
         <v>54</v>
       </c>
@@ -2091,7 +2095,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="44" t="s">
         <v>55</v>
       </c>
@@ -2102,7 +2106,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="44" t="s">
         <v>56</v>
       </c>
@@ -2113,7 +2117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="44" t="s">
         <v>57</v>
       </c>
@@ -2124,7 +2128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="44" t="s">
         <v>58</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="47" t="s">
         <v>66</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="47" t="s">
         <v>65</v>
       </c>
@@ -2157,7 +2161,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="25" t="s">
         <v>63</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="25" t="s">
         <v>64</v>
       </c>
@@ -2179,10 +2183,21 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <f>SUM(C3:C18)</f>
-        <v>4370</v>
+    <row r="19" spans="1:3">
+      <c r="A19" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="25">
+        <v>1</v>
+      </c>
+      <c r="C19" s="25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="C21">
+        <f>SUM(C3:C19)</f>
+        <v>4620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>